<commit_message>
1. Working api to read data from excel
</commit_message>
<xml_diff>
--- a/Calendar.xlsx
+++ b/Calendar.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Defect\TDD\calendar\calendar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\calendar-assistant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A62CDFA-5FC6-4132-B1A4-636B1AB958F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183F2620-F7C5-47DD-BCA5-29AAB5A3D1BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7FDEA331-AA49-46D1-8090-5CDB1A51D55C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{7FDEA331-AA49-46D1-8090-5CDB1A51D55C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="MEETING" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -427,17 +427,17 @@
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,7 +460,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44285</v>
       </c>

</xml_diff>